<commit_message>
Import Sutent base infomation and Thesis list.
</commit_message>
<xml_diff>
--- a/src/main/webapp/resources/template/excel/本科生-基本信息.xlsx
+++ b/src/main/webapp/resources/template/excel/本科生-基本信息.xlsx
@@ -30,15 +30,15 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>半价</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>性别</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>女</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>班级</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1006,7 +1006,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1022,10 +1022,10 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
@@ -1039,7 +1039,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>